<commit_message>
Added support for properties
</commit_message>
<xml_diff>
--- a/Assets/ExcelImporter/Example/Excels/MstItems.xlsx
+++ b/Assets/ExcelImporter/Example/Excels/MstItems.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">category</t>
   </si>
   <si>
+    <t xml:space="preserve">subIdsString</t>
+  </si>
+  <si>
     <t xml:space="preserve">The blank header cell means the end of the column</t>
   </si>
   <si>
@@ -52,27 +55,45 @@
     <t xml:space="preserve">Red</t>
   </si>
   <si>
+    <t xml:space="preserve">1,2,3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Base Factor ( Column 'E' = 'H3' * Column 'I' )</t>
   </si>
   <si>
     <t xml:space="preserve">item2</t>
   </si>
   <si>
+    <t xml:space="preserve">4,5,6</t>
+  </si>
+  <si>
     <t xml:space="preserve">item3</t>
   </si>
   <si>
+    <t xml:space="preserve">7,8,9</t>
+  </si>
+  <si>
     <t xml:space="preserve">item4</t>
   </si>
   <si>
     <t xml:space="preserve">Green</t>
   </si>
   <si>
+    <t xml:space="preserve">2,3,4</t>
+  </si>
+  <si>
     <t xml:space="preserve">item5</t>
   </si>
   <si>
+    <t xml:space="preserve">5,6,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">item6</t>
   </si>
   <si>
+    <t xml:space="preserve">6,7,8</t>
+  </si>
+  <si>
     <t xml:space="preserve"># This row is a comment.</t>
   </si>
   <si>
@@ -82,13 +103,25 @@
     <t xml:space="preserve">Blue</t>
   </si>
   <si>
+    <t xml:space="preserve">3,5,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">item8</t>
   </si>
   <si>
+    <t xml:space="preserve">1,5,7</t>
+  </si>
+  <si>
     <t xml:space="preserve">item9</t>
   </si>
   <si>
+    <t xml:space="preserve">2,4,9</t>
+  </si>
+  <si>
     <t xml:space="preserve">item10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2,4</t>
   </si>
   <si>
     <t xml:space="preserve">The first cell in the blank means the end of the row.</t>
@@ -105,7 +138,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -128,6 +161,12 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -225,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,6 +277,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,6 +317,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -286,15 +333,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -391,25 +438,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="45.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="12.42"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="17.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -428,307 +476,359 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="J1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="n">
+      <c r="A2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="n">
+        <f aca="false">$I$3*J2</f>
+        <v>2.3</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <f aca="false">$I$3*J3</f>
+        <v>3.22</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="12" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J3" s="11" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <f aca="false">$I$3*J4</f>
+        <v>3.68</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="11" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="14" t="n">
+        <v>60</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="n">
+        <f aca="false">$I$3*J5</f>
+        <v>4.14</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="11" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="14" t="n">
+        <v>180</v>
+      </c>
+      <c r="D6" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="14" t="n">
+        <f aca="false">$I$3*J6</f>
+        <v>4.83</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="11" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="14" t="n">
+        <v>230</v>
+      </c>
+      <c r="D7" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="14" t="n">
+        <f aca="false">$I$3*J7</f>
+        <v>5.06</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="20" t="n">
+        <v>310</v>
+      </c>
+      <c r="D9" s="21" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="20" t="n">
+        <f aca="false">$I$3*J9</f>
+        <v>5.52</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="7" t="b">
+      <c r="B10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="20" t="n">
+        <v>560</v>
+      </c>
+      <c r="D10" s="21" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="20" t="n">
+        <f aca="false">$I$3*J10</f>
+        <v>5.98</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="11" t="n">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="20" t="n">
+        <v>820</v>
+      </c>
+      <c r="D11" s="21" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="n">
-        <f aca="false">$H$3*I2</f>
-        <v>2.3</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="E11" s="20" t="n">
+        <f aca="false">$I$3*J11</f>
+        <v>6.44</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="11" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="I2" s="10" t="n">
+      <c r="B12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="20" t="n">
+        <v>1010</v>
+      </c>
+      <c r="D12" s="21" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6" t="n">
+      <c r="E12" s="20" t="n">
+        <f aca="false">$I$3*J12</f>
+        <v>8.05</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="11" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="n">
+        <v>99</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="23" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="18" t="n">
+        <f aca="false">$I$3*J15</f>
+        <v>22.77</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6" t="n">
-        <f aca="false">$H$3*I3</f>
-        <v>3.22</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="11" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="I3" s="10" t="n">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="D4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <f aca="false">$H$3*I4</f>
-        <v>3.68</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="10" t="n">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="12" t="n">
-        <v>60</v>
-      </c>
-      <c r="D5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="12" t="n">
-        <f aca="false">$H$3*I5</f>
-        <v>4.14</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="10" t="n">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="12" t="n">
-        <v>180</v>
-      </c>
-      <c r="D6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12" t="n">
-        <f aca="false">$H$3*I6</f>
-        <v>4.83</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="10" t="n">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="12" t="n">
-        <v>230</v>
-      </c>
-      <c r="D7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12" t="n">
-        <f aca="false">$H$3*I7</f>
-        <v>5.06</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="10" t="n">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="18" t="n">
-        <v>310</v>
-      </c>
-      <c r="D9" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="18" t="n">
-        <f aca="false">$H$3*I9</f>
-        <v>5.52</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="10" t="n">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="18" t="n">
-        <v>560</v>
-      </c>
-      <c r="D10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="18" t="n">
-        <f aca="false">$H$3*I10</f>
-        <v>5.98</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="10" t="n">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="18" t="n">
-        <v>820</v>
-      </c>
-      <c r="D11" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="18" t="n">
-        <f aca="false">$H$3*I11</f>
-        <v>6.44</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="10" t="n">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="18" t="n">
-        <v>1010</v>
-      </c>
-      <c r="D12" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="18" t="n">
-        <f aca="false">$H$3*I12</f>
-        <v>8.05</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="10" t="n">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="G15" s="18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="n">
-        <v>99</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="15" t="n">
-        <f aca="false">$H$3*I15</f>
-        <v>22.77</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="10" t="n">
+      <c r="J15" s="11" t="n">
         <v>9.9</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F2:F12" type="list">
       <formula1>"Red,Green,Blue"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D7 D9:D12" type="list">
       <formula1>"FALSE,TRUE"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G15" type="none">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>